<commit_message>
integrate xl to frame
</commit_message>
<xml_diff>
--- a/TestData/pyxlDemo.xlsx
+++ b/TestData/pyxlDemo.xlsx
@@ -11,15 +11,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Test Case</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>dob</t>
   </si>
   <si>
     <t>TC1</t>
@@ -28,24 +37,38 @@
     <t>Tester</t>
   </si>
   <si>
+    <t>qa@tester.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
     <t>TC2</t>
   </si>
   <si>
-    <t>QA</t>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>test@qa.com</t>
+  </si>
+  <si>
+    <t>test@1234</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
@@ -58,20 +81,31 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -300,21 +334,54 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2021993.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3021993.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>